<commit_message>
Implemented relative and absolute tolerances, ...
- String solutions are compared lowercase and stripped of space characters
- Updated template
- Applied a touch of blackness
</commit_message>
<xml_diff>
--- a/examples/exercise.xlsx
+++ b/examples/exercise.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Dropbox\2016 PyCor\PyCor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Python\PyCor-dev\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080623A0-76DC-4BD5-B9F4-433307204265}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="o4LZ7Fnl9RhEs6bNHdIpeBP7LR7QNq7WS7PPwHWEL/+ZxJNjetUjZABzsPLf2qMGF8DYoZX7ZoykzTgj4EPYAA==" workbookSaltValue="E7BU0C5z56PuDjyvUe/Lvw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Solution" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
   <si>
     <t>Matr. Nr.</t>
   </si>
@@ -51,9 +57,6 @@
     <t>Ru</t>
   </si>
   <si>
-    <t>Subject</t>
-  </si>
-  <si>
     <t>hm1</t>
   </si>
   <si>
@@ -102,37 +105,46 @@
     <t>Geschwindigkeit t</t>
   </si>
   <si>
-    <t>a1</t>
-  </si>
-  <si>
-    <t>a2</t>
-  </si>
-  <si>
-    <t>a3</t>
-  </si>
-  <si>
-    <t>a4</t>
-  </si>
-  <si>
-    <t>a5</t>
-  </si>
-  <si>
-    <t>a6</t>
-  </si>
-  <si>
-    <t>a7</t>
-  </si>
-  <si>
     <t>Exercise</t>
   </si>
   <si>
-    <t>not stabile</t>
+    <t>Titel</t>
+  </si>
+  <si>
+    <t>Auswahl 1</t>
+  </si>
+  <si>
+    <t>Auswahl 2</t>
+  </si>
+  <si>
+    <t>Auswahl 3</t>
+  </si>
+  <si>
+    <t>Auswahl 4</t>
+  </si>
+  <si>
+    <t>Auswahl 5</t>
+  </si>
+  <si>
+    <t>Auswahl 6</t>
+  </si>
+  <si>
+    <t>Auswahl 7</t>
+  </si>
+  <si>
+    <t>Wert</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>Nicht korrigiert</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -176,7 +188,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -212,34 +224,10 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -249,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -257,12 +245,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -573,99 +568,155 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="12.875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.125" style="1"/>
+    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="1" customWidth="1"/>
+    <col min="4" max="7" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="8" spans="1:8" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1.56</v>
+      </c>
+      <c r="C9" s="5">
+        <v>-2</v>
+      </c>
+      <c r="D9" s="5">
+        <v>20</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B10" s="9">
         <v>4412670</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="7">
-        <v>1.56</v>
-      </c>
-      <c r="B6" s="8">
-        <v>-2</v>
-      </c>
-      <c r="C6" s="8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="3">
+        <v>12.5</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>1</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="3">
+        <v>16.3</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="3">
+        <v>5</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="3">
+        <v>6</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="9"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
-        <v>1</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -673,13 +724,13 @@
         <v>1</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C17" s="3">
-        <v>1.25</v>
+        <v>7</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -687,13 +738,13 @@
         <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C18" s="3">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -701,10 +752,10 @@
         <v>1</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
+      </c>
+      <c r="C19" s="3">
+        <v>18</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>21</v>
@@ -715,50 +766,52 @@
         <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2</v>
+      </c>
       <c r="D20" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C21" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C22" s="3">
-        <v>4</v>
+        <v>1.2</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C23" s="3">
-        <v>3.2450000000000001</v>
+        <v>1.5</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>21</v>
@@ -769,78 +822,67 @@
         <v>2</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="C24" s="3">
+        <v>1.7</v>
+      </c>
       <c r="D24" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
+        <v>3</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="3">
         <v>2</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="C26" s="3">
+        <v>8</v>
+      </c>
       <c r="D26" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="C27" s="3"/>
-      <c r="D27" s="3" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C28" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
-        <v>3</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29" s="3">
-        <v>3.75</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated example files and manual
</commit_message>
<xml_diff>
--- a/examples/exercise.xlsx
+++ b/examples/exercise.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Python\PyCor-dev\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080623A0-76DC-4BD5-B9F4-433307204265}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5129986A-E0BF-4A40-85F0-BEE529F8E731}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="o4LZ7Fnl9RhEs6bNHdIpeBP7LR7QNq7WS7PPwHWEL/+ZxJNjetUjZABzsPLf2qMGF8DYoZX7ZoykzTgj4EPYAA==" workbookSaltValue="E7BU0C5z56PuDjyvUe/Lvw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Solution" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>Matr. Nr.</t>
   </si>
@@ -139,6 +140,9 @@
   </si>
   <si>
     <t>Nicht korrigiert</t>
+  </si>
+  <si>
+    <t>Auswahl 8</t>
   </si>
 </sst>
 </file>
@@ -257,7 +261,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -569,13 +573,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="21.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -584,7 +588,7 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -597,7 +601,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="8" spans="1:8" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>2</v>
       </c>
@@ -622,8 +626,11 @@
       <c r="H8" s="8" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I8" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>33</v>
       </c>
@@ -640,8 +647,9 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
@@ -649,7 +657,7 @@
         <v>4412670</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>24</v>
       </c>
@@ -663,7 +671,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>1</v>
       </c>
@@ -677,7 +685,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>1</v>
       </c>
@@ -691,7 +699,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>1</v>
       </c>
@@ -705,7 +713,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>1</v>
       </c>

</xml_diff>